<commit_message>
a good new chunk of numbers, really starting to speed this up.
</commit_message>
<xml_diff>
--- a/DavidLynchWeatherTracking.xlsx
+++ b/DavidLynchWeatherTracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="19100" windowHeight="7300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
   <si>
     <t>David Lynch Talking Weather Clock</t>
   </si>
@@ -265,6 +265,69 @@
   </si>
   <si>
     <t>haveagreatday</t>
+  </si>
+  <si>
+    <t>on christmas, christmas message after current temps</t>
+  </si>
+  <si>
+    <t>From memory format</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>[it's date]</t>
+  </si>
+  <si>
+    <t>[year]</t>
+  </si>
+  <si>
+    <t>here in</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>tempf</t>
+  </si>
+  <si>
+    <t>degreesf</t>
+  </si>
+  <si>
+    <t>tempc</t>
+  </si>
+  <si>
+    <t>degreesc</t>
+  </si>
+  <si>
+    <t>wind conditions</t>
+  </si>
+  <si>
+    <t>later</t>
+  </si>
+  <si>
+    <t>should go [up or down]</t>
+  </si>
+  <si>
+    <t>forecastf</t>
+  </si>
+  <si>
+    <t>forecastc</t>
+  </si>
+  <si>
+    <t>(Good morning or afternoon/evening)</t>
+  </si>
+  <si>
+    <t>and it's a [day of the week]</t>
+  </si>
+  <si>
+    <t>MUSIC thinking about</t>
+  </si>
+  <si>
+    <t>blue skies</t>
+  </si>
+  <si>
+    <t>have a great day</t>
   </si>
 </sst>
 </file>
@@ -3370,90 +3433,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>726</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -3500,12 +3566,130 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>